<commit_message>
Minor change to fix calculate_make_miss_playoffs, was doing it backwards by accident
</commit_message>
<xml_diff>
--- a/fantasy_league_stats_new_output.xlsx
+++ b/fantasy_league_stats_new_output.xlsx
@@ -14,7 +14,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="47">
+  <si>
+    <t>Year</t>
+  </si>
   <si>
     <t>Aaron</t>
   </si>
@@ -46,37 +49,112 @@
     <t>Liam W</t>
   </si>
   <si>
-    <t>2014</t>
-  </si>
-  <si>
-    <t>2015</t>
-  </si>
-  <si>
-    <t>2016</t>
-  </si>
-  <si>
-    <t>2017</t>
-  </si>
-  <si>
-    <t>2018</t>
-  </si>
-  <si>
-    <t>2019</t>
-  </si>
-  <si>
-    <t>2020</t>
-  </si>
-  <si>
-    <t>2021</t>
-  </si>
-  <si>
-    <t>2022</t>
-  </si>
-  <si>
-    <t>2023</t>
-  </si>
-  <si>
-    <t>2024</t>
+    <t>8-6-0</t>
+  </si>
+  <si>
+    <t>7-7-0</t>
+  </si>
+  <si>
+    <t>6-8-0</t>
+  </si>
+  <si>
+    <t>3-11-0</t>
+  </si>
+  <si>
+    <t>9-5-0</t>
+  </si>
+  <si>
+    <t>Overall</t>
+  </si>
+  <si>
+    <t>73-85-0</t>
+  </si>
+  <si>
+    <t>85-72-1</t>
+  </si>
+  <si>
+    <t>72-58-0</t>
+  </si>
+  <si>
+    <t>81-77-0</t>
+  </si>
+  <si>
+    <t>67-91-0</t>
+  </si>
+  <si>
+    <t>66-64-0</t>
+  </si>
+  <si>
+    <t>75-83-0</t>
+  </si>
+  <si>
+    <t>78-80-0</t>
+  </si>
+  <si>
+    <t>91-66-1</t>
+  </si>
+  <si>
+    <t>12-2-0</t>
+  </si>
+  <si>
+    <t>5-9-0</t>
+  </si>
+  <si>
+    <t>11-3-0</t>
+  </si>
+  <si>
+    <t>1-13-0</t>
+  </si>
+  <si>
+    <t>9-4-1</t>
+  </si>
+  <si>
+    <t>6-7-1</t>
+  </si>
+  <si>
+    <t>4-10-0</t>
+  </si>
+  <si>
+    <t>2-12-0</t>
+  </si>
+  <si>
+    <t>10-4-0</t>
+  </si>
+  <si>
+    <t>13-1-0</t>
+  </si>
+  <si>
+    <t>11-4-0</t>
+  </si>
+  <si>
+    <t>7-8-0</t>
+  </si>
+  <si>
+    <t>4-11-0</t>
+  </si>
+  <si>
+    <t>10-5-0</t>
+  </si>
+  <si>
+    <t>6-9-0</t>
+  </si>
+  <si>
+    <t>8-7-0</t>
+  </si>
+  <si>
+    <t>5-10-0</t>
+  </si>
+  <si>
+    <t>9-6-0</t>
+  </si>
+  <si>
+    <t>2-13-0</t>
+  </si>
+  <si>
+    <t>12-3-0</t>
+  </si>
+  <si>
+    <t>3-12-0</t>
   </si>
 </sst>
 </file>
@@ -411,105 +489,458 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P15"/>
+  <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="16" width="6.85546875" style="1" customWidth="1"/>
+    <col min="1" max="11" width="12.85546875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="1" customFormat="1" ht="18" customHeight="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:11" s="1" customFormat="1" ht="18" customHeight="1">
-      <c r="A2" s="1" t="s">
-        <v>10</v>
+      <c r="A2" s="1">
+        <v>2014</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:11" s="1" customFormat="1" ht="18" customHeight="1">
-      <c r="A3" s="1" t="s">
-        <v>11</v>
+      <c r="A3" s="1">
+        <v>2015</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:11" s="1" customFormat="1" ht="18" customHeight="1">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="1">
+        <v>2016</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" s="1" customFormat="1" ht="18" customHeight="1">
+      <c r="A5" s="1">
+        <v>2017</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I5" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" s="1" customFormat="1" ht="18" customHeight="1">
-      <c r="A5" s="1" t="s">
+      <c r="J5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" s="1" customFormat="1" ht="18" customHeight="1">
+      <c r="A6" s="1">
+        <v>2018</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" s="1" customFormat="1" ht="18" customHeight="1">
+      <c r="A7" s="1">
+        <v>2019</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I7" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" s="1" customFormat="1" ht="18" customHeight="1">
-      <c r="A6" s="1" t="s">
+      <c r="J7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" s="1" customFormat="1" ht="18" customHeight="1">
+      <c r="A8" s="1">
+        <v>2020</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F8" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" s="1" customFormat="1" ht="18" customHeight="1">
-      <c r="A7" s="1" t="s">
+      <c r="G8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="I8" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" s="1" customFormat="1" ht="18" customHeight="1">
-      <c r="A8" s="1" t="s">
+      <c r="J8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" s="1" customFormat="1" ht="18" customHeight="1">
+      <c r="A9" s="1">
+        <v>2021</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" s="1" customFormat="1" ht="18" customHeight="1">
+      <c r="A10" s="1">
+        <v>2022</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" s="1" customFormat="1" ht="18" customHeight="1">
+      <c r="A11" s="1">
+        <v>2023</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" s="1" customFormat="1" ht="18" customHeight="1">
+      <c r="A12" s="1">
+        <v>2024</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="A13" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" s="1" customFormat="1" ht="18" customHeight="1">
-      <c r="A9" s="1" t="s">
+      <c r="B13" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" s="1" customFormat="1" ht="18" customHeight="1">
-      <c r="A10" s="1" t="s">
+      <c r="C13" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" s="1" customFormat="1" ht="18" customHeight="1">
-      <c r="A11" s="1" t="s">
+      <c r="D13" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" s="1" customFormat="1" ht="18" customHeight="1">
-      <c r="A12" s="1" t="s">
+      <c r="E13" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" s="1" customFormat="1" ht="18" customHeight="1"/>
-    <row r="14" spans="1:11" s="1" customFormat="1" ht="18" customHeight="1"/>
-    <row r="15" spans="1:11" s="1" customFormat="1" ht="18" customHeight="1"/>
+      <c r="F13" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Done! Created all 10 conventional Excel Worksheets
</commit_message>
<xml_diff>
--- a/fantasy_league_stats_new_output.xlsx
+++ b/fantasy_league_stats_new_output.xlsx
@@ -14,7 +14,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="47">
+  <si>
+    <t>Year</t>
+  </si>
   <si>
     <t>Aaron</t>
   </si>
@@ -46,37 +49,112 @@
     <t>Liam W</t>
   </si>
   <si>
-    <t>2014</t>
-  </si>
-  <si>
-    <t>2015</t>
-  </si>
-  <si>
-    <t>2016</t>
-  </si>
-  <si>
-    <t>2017</t>
-  </si>
-  <si>
-    <t>2018</t>
-  </si>
-  <si>
-    <t>2019</t>
-  </si>
-  <si>
-    <t>2020</t>
-  </si>
-  <si>
-    <t>2021</t>
-  </si>
-  <si>
-    <t>2022</t>
-  </si>
-  <si>
-    <t>2023</t>
-  </si>
-  <si>
-    <t>2024</t>
+    <t>8-6-0</t>
+  </si>
+  <si>
+    <t>7-7-0</t>
+  </si>
+  <si>
+    <t>6-8-0</t>
+  </si>
+  <si>
+    <t>3-11-0</t>
+  </si>
+  <si>
+    <t>9-5-0</t>
+  </si>
+  <si>
+    <t>Overall</t>
+  </si>
+  <si>
+    <t>73-85-0</t>
+  </si>
+  <si>
+    <t>85-72-1</t>
+  </si>
+  <si>
+    <t>72-58-0</t>
+  </si>
+  <si>
+    <t>81-77-0</t>
+  </si>
+  <si>
+    <t>67-91-0</t>
+  </si>
+  <si>
+    <t>66-64-0</t>
+  </si>
+  <si>
+    <t>75-83-0</t>
+  </si>
+  <si>
+    <t>78-80-0</t>
+  </si>
+  <si>
+    <t>91-66-1</t>
+  </si>
+  <si>
+    <t>12-2-0</t>
+  </si>
+  <si>
+    <t>5-9-0</t>
+  </si>
+  <si>
+    <t>11-3-0</t>
+  </si>
+  <si>
+    <t>1-13-0</t>
+  </si>
+  <si>
+    <t>9-4-1</t>
+  </si>
+  <si>
+    <t>6-7-1</t>
+  </si>
+  <si>
+    <t>4-10-0</t>
+  </si>
+  <si>
+    <t>2-12-0</t>
+  </si>
+  <si>
+    <t>10-4-0</t>
+  </si>
+  <si>
+    <t>13-1-0</t>
+  </si>
+  <si>
+    <t>11-4-0</t>
+  </si>
+  <si>
+    <t>7-8-0</t>
+  </si>
+  <si>
+    <t>4-11-0</t>
+  </si>
+  <si>
+    <t>10-5-0</t>
+  </si>
+  <si>
+    <t>6-9-0</t>
+  </si>
+  <si>
+    <t>8-7-0</t>
+  </si>
+  <si>
+    <t>5-10-0</t>
+  </si>
+  <si>
+    <t>9-6-0</t>
+  </si>
+  <si>
+    <t>2-13-0</t>
+  </si>
+  <si>
+    <t>12-3-0</t>
+  </si>
+  <si>
+    <t>3-12-0</t>
   </si>
 </sst>
 </file>
@@ -411,105 +489,458 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P15"/>
+  <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="16" width="6.85546875" style="1" customWidth="1"/>
+    <col min="1" max="11" width="12.85546875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="1" customFormat="1" ht="18" customHeight="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:11" s="1" customFormat="1" ht="18" customHeight="1">
-      <c r="A2" s="1" t="s">
-        <v>10</v>
+      <c r="A2" s="1">
+        <v>2014</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:11" s="1" customFormat="1" ht="18" customHeight="1">
-      <c r="A3" s="1" t="s">
-        <v>11</v>
+      <c r="A3" s="1">
+        <v>2015</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:11" s="1" customFormat="1" ht="18" customHeight="1">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="1">
+        <v>2016</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" s="1" customFormat="1" ht="18" customHeight="1">
+      <c r="A5" s="1">
+        <v>2017</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I5" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" s="1" customFormat="1" ht="18" customHeight="1">
-      <c r="A5" s="1" t="s">
+      <c r="J5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" s="1" customFormat="1" ht="18" customHeight="1">
+      <c r="A6" s="1">
+        <v>2018</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" s="1" customFormat="1" ht="18" customHeight="1">
+      <c r="A7" s="1">
+        <v>2019</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I7" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" s="1" customFormat="1" ht="18" customHeight="1">
-      <c r="A6" s="1" t="s">
+      <c r="J7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" s="1" customFormat="1" ht="18" customHeight="1">
+      <c r="A8" s="1">
+        <v>2020</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F8" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" s="1" customFormat="1" ht="18" customHeight="1">
-      <c r="A7" s="1" t="s">
+      <c r="G8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="I8" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" s="1" customFormat="1" ht="18" customHeight="1">
-      <c r="A8" s="1" t="s">
+      <c r="J8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" s="1" customFormat="1" ht="18" customHeight="1">
+      <c r="A9" s="1">
+        <v>2021</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" s="1" customFormat="1" ht="18" customHeight="1">
+      <c r="A10" s="1">
+        <v>2022</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" s="1" customFormat="1" ht="18" customHeight="1">
+      <c r="A11" s="1">
+        <v>2023</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" s="1" customFormat="1" ht="18" customHeight="1">
+      <c r="A12" s="1">
+        <v>2024</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="A13" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" s="1" customFormat="1" ht="18" customHeight="1">
-      <c r="A9" s="1" t="s">
+      <c r="B13" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" s="1" customFormat="1" ht="18" customHeight="1">
-      <c r="A10" s="1" t="s">
+      <c r="C13" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" s="1" customFormat="1" ht="18" customHeight="1">
-      <c r="A11" s="1" t="s">
+      <c r="D13" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" s="1" customFormat="1" ht="18" customHeight="1">
-      <c r="A12" s="1" t="s">
+      <c r="E13" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" s="1" customFormat="1" ht="18" customHeight="1"/>
-    <row r="14" spans="1:11" s="1" customFormat="1" ht="18" customHeight="1"/>
-    <row r="15" spans="1:11" s="1" customFormat="1" ht="18" customHeight="1"/>
+      <c r="F13" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>